<commit_message>
subiendo cambios en segunda rama
</commit_message>
<xml_diff>
--- a/P1G1/CRONOGRAMA.xlsx
+++ b/P1G1/CRONOGRAMA.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="49">
   <si>
     <t>LUIS LEE</t>
   </si>
@@ -80,13 +80,100 @@
   </si>
   <si>
     <t>Login mantenimientos</t>
+  </si>
+  <si>
+    <t>Luis Carlos Lee</t>
+  </si>
+  <si>
+    <t>Alumno</t>
+  </si>
+  <si>
+    <t>Trabajo</t>
+  </si>
+  <si>
+    <t>Especificacion</t>
+  </si>
+  <si>
+    <t>Secciones, sedes, aulas, jornadas</t>
+  </si>
+  <si>
+    <t>Fernando Tobar</t>
+  </si>
+  <si>
+    <t>Jose Jeronimo</t>
+  </si>
+  <si>
+    <t>Emerson Miranda</t>
+  </si>
+  <si>
+    <t>Nayre de Leon</t>
+  </si>
+  <si>
+    <t>Carlos Castillo</t>
+  </si>
+  <si>
+    <t>Alumnos, maestros, facultades, carreras, cursos</t>
+  </si>
+  <si>
+    <t>Asignacion de cursos</t>
+  </si>
+  <si>
+    <t>alumnos.</t>
+  </si>
+  <si>
+    <t>maestros + notas</t>
+  </si>
+  <si>
+    <t>login admin</t>
+  </si>
+  <si>
+    <t>login que permite crear usuarios y ver todo lo demas</t>
+  </si>
+  <si>
+    <t>login asignacion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">login que permite asignar cursos </t>
+  </si>
+  <si>
+    <t>Funciona</t>
+  </si>
+  <si>
+    <t>si</t>
+  </si>
+  <si>
+    <t>no entrego</t>
+  </si>
+  <si>
+    <t>tira error de sql</t>
+  </si>
+  <si>
+    <t>tiene errores</t>
+  </si>
+  <si>
+    <t>no deja fusionar</t>
+  </si>
+  <si>
+    <t>Gustavo Jax</t>
+  </si>
+  <si>
+    <t>login mantenimientos</t>
+  </si>
+  <si>
+    <t>manteniminetos</t>
+  </si>
+  <si>
+    <t>mantenimientos</t>
+  </si>
+  <si>
+    <t>login que permite ver mantenimientos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -109,8 +196,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -126,6 +219,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -194,7 +293,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -242,6 +341,12 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -516,7 +621,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -524,18 +629,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:O16"/>
+  <dimension ref="B1:O25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="48.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15" style="1" customWidth="1"/>
     <col min="8" max="8" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
@@ -629,7 +734,9 @@
       <c r="D7" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="16"/>
+      <c r="E7" s="16" t="s">
+        <v>5</v>
+      </c>
       <c r="F7" s="16" t="s">
         <v>14</v>
       </c>
@@ -686,13 +793,13 @@
         <v>0</v>
       </c>
       <c r="G9" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9" s="9" t="s">
         <v>8</v>
       </c>
       <c r="I9" s="15">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="J9" s="11"/>
       <c r="K9" s="13"/>
@@ -707,7 +814,9 @@
       <c r="D10" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="7"/>
+      <c r="E10" s="16" t="s">
+        <v>5</v>
+      </c>
       <c r="F10" s="7" t="s">
         <v>14</v>
       </c>
@@ -764,7 +873,7 @@
         <v>6</v>
       </c>
       <c r="G12" s="15">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>9</v>
@@ -784,7 +893,9 @@
       <c r="D13" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="E13" s="7"/>
+      <c r="E13" s="16" t="s">
+        <v>5</v>
+      </c>
       <c r="F13" s="7" t="s">
         <v>14</v>
       </c>
@@ -825,7 +936,7 @@
         <v>11</v>
       </c>
       <c r="I14" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J14" s="6" t="s">
         <v>12</v>
@@ -849,13 +960,13 @@
         <v>10</v>
       </c>
       <c r="G15" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I15" s="15">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="J15" s="6" t="s">
         <v>12</v>
@@ -865,14 +976,133 @@
       </c>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="F16" s="1" t="s">
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="G16" s="3"/>
+      <c r="H16" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="J16" t="s">
+      <c r="I16" s="3"/>
+      <c r="J16" s="5" t="s">
         <v>19</v>
+      </c>
+      <c r="K16" s="5"/>
+    </row>
+    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C18" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="F18" s="26" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C19" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C20" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C21" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C22" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C23" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C24" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C25" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>